<commit_message>
Refactoring: RandomVariable and other Monte-Carlo components.
Refactoring of names. Interfaces come with plain names
	RandomVariable
while implementation come with implementation details
	RandomVariableFromDouleArray.
</commit_message>
<xml_diff>
--- a/doc/refactoring-3.6.x-to-4.0.0/Refactorings 3.6.x to 4.0.0.xlsx
+++ b/doc/refactoring-3.6.x-to-4.0.0/Refactorings 3.6.x to 4.0.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fries/Documents/Development/Repositories/finmath lib/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fries/Documents/Development/Repositories/finmath lib/doc/refactoring-3.6.x-to-4.0.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3AE8BB-273D-1043-A9B5-702CFF518CEE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AA3E67-F968-064A-8A95-C10F6D31E960}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20000" xr2:uid="{89A50B95-A836-9647-8368-30876D9BFE05}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="145">
   <si>
     <t>method</t>
   </si>
@@ -327,9 +327,6 @@
     <t>RandomVariableDifferentiableInterface</t>
   </si>
   <si>
-    <t>RandomVariableValueDouble</t>
-  </si>
-  <si>
     <t>RandomVariable</t>
   </si>
   <si>
@@ -553,13 +550,22 @@
   </si>
   <si>
     <t>CalibrationProduct[] should be used instead of three parameters in some methods</t>
+  </si>
+  <si>
+    <t>RandomVariableFromDoubleArray</t>
+  </si>
+  <si>
+    <t>RandomVariableLowMemory</t>
+  </si>
+  <si>
+    <t>RandomVariableFromFloatArray</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -601,8 +607,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -612,6 +624,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -646,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -658,6 +676,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -972,871 +991,894 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6EACCA-7E26-C148-ACB1-915E31E23464}">
-  <dimension ref="A1:E125"/>
+  <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A126" sqref="A126"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="66.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" customWidth="1"/>
-    <col min="4" max="4" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="3" width="66.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="9" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>133</v>
-      </c>
+    <row r="1" spans="2:6" s="9" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="10" t="s">
         <v>132</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>130</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
+      <c r="F1" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="2"/>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="C3" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>127</v>
-      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="C5" t="s">
         <v>125</v>
       </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C6" s="5" t="s">
         <v>123</v>
       </c>
+      <c r="D6" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
         <v>122</v>
       </c>
+      <c r="C7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>121</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="C8" t="s">
         <v>120</v>
       </c>
+      <c r="D8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>118</v>
-      </c>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="C10" t="s">
         <v>116</v>
       </c>
+      <c r="D10" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="C11" s="5" t="s">
         <v>114</v>
       </c>
+      <c r="D11" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="C12" t="s">
         <v>112</v>
       </c>
+      <c r="D12" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="C13" s="5" t="s">
         <v>110</v>
       </c>
+      <c r="D13" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="C14" t="s">
         <v>108</v>
       </c>
+      <c r="D14" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="C15" s="5" t="s">
         <v>106</v>
       </c>
+      <c r="D15" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>105</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="C16" t="s">
         <v>104</v>
       </c>
+      <c r="D16" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="C17" t="s">
         <v>102</v>
       </c>
+      <c r="D17" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>100</v>
       </c>
+      <c r="D18" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>98</v>
       </c>
+      <c r="D19" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="C20" s="6" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="D20" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="2" t="s">
         <v>95</v>
       </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C24" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="D24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
         <v>92</v>
       </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="C25" t="s">
         <v>90</v>
       </c>
+      <c r="D25" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>88</v>
-      </c>
+    <row r="27" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
         <v>87</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>86</v>
-      </c>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+      <c r="C29" t="s">
         <v>84</v>
       </c>
+      <c r="D29" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
         <v>83</v>
       </c>
       <c r="C30" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="32" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" t="s">
         <v>138</v>
       </c>
-      <c r="B34" t="s">
-        <v>139</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>81</v>
-      </c>
+      <c r="D34" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>80</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="C36" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="D36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" t="s">
         <v>78</v>
       </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>76</v>
-      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>75</v>
       </c>
       <c r="C38" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>74</v>
-      </c>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="C40" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="D40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" t="s">
         <v>71</v>
       </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C41" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="43" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="11"/>
+      <c r="B43" s="2" t="s">
         <v>69</v>
       </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="11"/>
       <c r="B45" t="s">
         <v>68</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>68</v>
-      </c>
+      <c r="C45" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="11"/>
       <c r="B46" t="s">
         <v>67</v>
       </c>
       <c r="C46" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="11"/>
+      <c r="B47" t="s">
+        <v>143</v>
+      </c>
+      <c r="C47" t="s">
+        <v>144</v>
+      </c>
+      <c r="D47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="11"/>
+      <c r="B48" t="s">
         <v>66</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C48" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="D48" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="11"/>
+      <c r="B50" t="s">
         <v>64</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C50" t="s">
         <v>63</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="D50" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="11"/>
+      <c r="B51" t="s">
         <v>63</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C51" t="s">
         <v>62</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D51" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="11"/>
+      <c r="B52" t="s">
         <v>61</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C52" t="s">
         <v>60</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="D52" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="11"/>
+      <c r="B53" t="s">
         <v>60</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C53" t="s">
         <v>59</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D53" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="11"/>
+      <c r="B55" t="s">
         <v>58</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C55" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
+      <c r="D55" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
         <v>55</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C59" t="s">
         <v>54</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="D59" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
         <v>53</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C61" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="D61" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
         <v>52</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C62" t="s">
         <v>51</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D62" t="s">
         <v>15</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E62" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
         <v>49</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C64" t="s">
         <v>50</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="D64" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
         <v>49</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C65" t="s">
         <v>48</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D65" t="s">
         <v>15</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E65" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
         <v>46</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C67" t="s">
         <v>45</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="D67" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
         <v>45</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C68" t="s">
         <v>44</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D68" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
         <v>43</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C70" t="s">
         <v>42</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="D70" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
         <v>42</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C71" t="s">
         <v>41</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D71" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
         <v>40</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C73" t="s">
         <v>39</v>
       </c>
-      <c r="C72" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="D73" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
         <v>39</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C74" t="s">
         <v>38</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D74" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
         <v>37</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C76" t="s">
         <v>36</v>
       </c>
-      <c r="C75" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="D76" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
         <v>35</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C78" t="s">
         <v>34</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+      <c r="D78" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
         <v>33</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C79" t="s">
         <v>32</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="D79" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
         <v>31</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C80" t="s">
         <v>30</v>
       </c>
-      <c r="C79" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="D80" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
         <v>29</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C81" t="s">
         <v>28</v>
       </c>
-      <c r="C80" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="2" t="s">
+      <c r="D81" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B83" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B85" t="s">
         <v>26</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C85" t="s">
         <v>25</v>
       </c>
-      <c r="C84" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+      <c r="D85" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B86" t="s">
         <v>24</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C86" t="s">
         <v>23</v>
       </c>
-      <c r="C85" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+      <c r="D86" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
         <v>23</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C87" t="s">
         <v>22</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D87" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
         <v>21</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C88" t="s">
         <v>20</v>
       </c>
-      <c r="C87" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+      <c r="D88" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
         <v>20</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C89" t="s">
         <v>19</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D89" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B90" t="s">
         <v>18</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C90" t="s">
         <v>17</v>
       </c>
-      <c r="C89" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+      <c r="D90" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
         <v>17</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C91" t="s">
         <v>16</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D91" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B92" t="s">
         <v>14</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C92" t="s">
         <v>13</v>
       </c>
-      <c r="C91" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>11</v>
-      </c>
-      <c r="B97" t="s">
-        <v>12</v>
-      </c>
-      <c r="C97" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>11</v>
-      </c>
+      <c r="D92" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>11</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="C98" t="s">
+        <v>12</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B99" t="s">
+        <v>11</v>
+      </c>
+      <c r="C99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D99" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>8</v>
-      </c>
-      <c r="B100" t="s">
-        <v>10</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>8</v>
-      </c>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>8</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="C101" t="s">
+        <v>10</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B102" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" t="s">
+        <v>8</v>
+      </c>
+      <c r="D102" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C102" s="3"/>
-    </row>
-    <row r="103" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="2" t="s">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D103" s="3"/>
+    </row>
+    <row r="104" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B104" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
         <v>5</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C106" t="s">
         <v>4</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D106" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B106" t="s">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C107" t="s">
         <v>3</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D107" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
         <v>2</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C109" t="s">
         <v>1</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D109" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B109" t="s">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C110" t="s">
+        <v>133</v>
+      </c>
+      <c r="D110" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B118" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C109" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="2" t="s">
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" s="11"/>
+      <c r="B120" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
+      <c r="C120" t="s">
         <v>136</v>
       </c>
-      <c r="B119" t="s">
-        <v>137</v>
-      </c>
-      <c r="C119" t="s">
+      <c r="D120" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="2" t="s">
+    <row r="123" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B123" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B125" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B126" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring: Models and Products.
Refactoring of names. Interfaces come with plain names
	Model, Product, TermStructureModel, LIBORModel
while implementation come with implementation details
	LIBORModelFromCovarianceModel
</commit_message>
<xml_diff>
--- a/doc/refactoring-3.6.x-to-4.0.0/Refactorings 3.6.x to 4.0.0.xlsx
+++ b/doc/refactoring-3.6.x-to-4.0.0/Refactorings 3.6.x to 4.0.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fries/Documents/Development/Repositories/finmath lib/doc/refactoring-3.6.x-to-4.0.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AA3E67-F968-064A-8A95-C10F6D31E960}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF49A44-2B26-2242-869E-AAFA4254D1C8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20000" xr2:uid="{89A50B95-A836-9647-8368-30876D9BFE05}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="153">
   <si>
     <t>method</t>
   </si>
@@ -560,12 +560,36 @@
   <si>
     <t>RandomVariableFromFloatArray</t>
   </si>
+  <si>
+    <t>TimeDiscretization and other time concepts</t>
+  </si>
+  <si>
+    <t>Optimizers</t>
+  </si>
+  <si>
+    <t>net.finmath.montecarlo.model</t>
+  </si>
+  <si>
+    <t>net.finmath.montecarlo.process</t>
+  </si>
+  <si>
+    <t>net.finmath.modelling</t>
+  </si>
+  <si>
+    <t>net.finmath.montecarlo</t>
+  </si>
+  <si>
+    <t>net.finmath.montecarlo.assetderivativevaluation.products</t>
+  </si>
+  <si>
+    <t>net.finmath.montecarlo.assetderivativevaluation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -612,6 +636,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Monaco"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -664,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -677,6 +707,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -991,893 +1022,986 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6EACCA-7E26-C148-ACB1-915E31E23464}">
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.5" customWidth="1"/>
-    <col min="2" max="3" width="66.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" customWidth="1"/>
-    <col min="5" max="5" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="4" width="66.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+    <col min="6" max="6" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="9" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:7" s="9" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="E3" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" t="s">
         <v>126</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>125</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="5" t="s">
+      <c r="E5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="E6" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
         <v>122</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+      <c r="E7" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
         <v>121</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>120</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="5" t="s">
+      <c r="E8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" t="s">
         <v>117</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>116</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="5" t="s">
+      <c r="E10" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+      <c r="E11" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" t="s">
         <v>113</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>112</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E12" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11"/>
       <c r="B13" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+      <c r="E13" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
         <v>109</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="5" t="s">
+      <c r="E14" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+      <c r="E15" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
         <v>105</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+      <c r="E16" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
         <v>103</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>102</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="5" t="s">
+      <c r="E17" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="6" t="s">
+      <c r="E18" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="6" t="s">
+      <c r="E19" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="2" t="s">
+      <c r="E20" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="11"/>
+      <c r="B24" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24" t="s">
         <v>94</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="E24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="11"/>
+      <c r="B25" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C25" t="s">
         <v>91</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
+      <c r="E25" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="11"/>
+      <c r="B26" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" t="s">
         <v>89</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>88</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="5" t="s">
+    <row r="27" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11"/>
+      <c r="B27" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="11"/>
+      <c r="B29" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C29" t="s">
         <v>85</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="5" t="s">
+      <c r="E29" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="11"/>
+      <c r="B30" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="2" t="s">
+    <row r="32" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
         <v>137</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>138</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
+      <c r="E34" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
         <v>80</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>79</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="E36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
         <v>77</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="E37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
         <v>75</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>74</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
         <v>73</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>72</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="E40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>70</v>
-      </c>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
         <v>70</v>
       </c>
       <c r="D41" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11"/>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="11"/>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>68</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E45" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>67</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>142</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="11"/>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>143</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>144</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>66</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>65</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E48" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="11"/>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>64</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>63</v>
       </c>
-      <c r="D50" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E50" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="11"/>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>63</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>62</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="11"/>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>61</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>60</v>
       </c>
-      <c r="D52" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E52" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="11"/>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>60</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>59</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="11"/>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>58</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>57</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="2" t="s">
+      <c r="E55" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="11"/>
+      <c r="C59" t="s">
         <v>55</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>54</v>
       </c>
-      <c r="D59" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
+      <c r="E59" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="2"/>
+      <c r="C61" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="11"/>
+      <c r="C63" t="s">
         <v>53</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D63" t="s">
         <v>52</v>
       </c>
-      <c r="D61" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B62" t="s">
+      <c r="E63" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="11"/>
+      <c r="C64" t="s">
         <v>52</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D64" t="s">
         <v>51</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E64" t="s">
         <v>15</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F64" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="11"/>
+      <c r="C66" t="s">
         <v>49</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D66" t="s">
         <v>50</v>
       </c>
-      <c r="D64" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
+      <c r="E66" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="11"/>
+      <c r="C67" t="s">
         <v>49</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D67" t="s">
         <v>48</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E67" t="s">
         <v>15</v>
       </c>
-      <c r="E65" t="s">
+      <c r="F67" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="11"/>
+      <c r="C69" t="s">
         <v>46</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D69" t="s">
         <v>45</v>
       </c>
-      <c r="D67" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
+      <c r="E69" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="11"/>
+      <c r="C70" t="s">
         <v>45</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D70" t="s">
         <v>44</v>
       </c>
-      <c r="D68" t="s">
+      <c r="E70" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B70" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="11"/>
+      <c r="C72" t="s">
         <v>43</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D72" t="s">
         <v>42</v>
       </c>
-      <c r="D70" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B71" t="s">
+      <c r="E72" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="11"/>
+      <c r="C73" t="s">
         <v>42</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D73" t="s">
         <v>41</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E73" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B73" t="s">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="11"/>
+      <c r="C75" t="s">
         <v>40</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D75" t="s">
         <v>39</v>
       </c>
-      <c r="D73" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B74" t="s">
+      <c r="E75" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="11"/>
+      <c r="C76" t="s">
         <v>39</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D76" t="s">
         <v>38</v>
       </c>
-      <c r="D74" t="s">
+      <c r="E76" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B76" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="11"/>
+      <c r="C78" t="s">
         <v>37</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D78" t="s">
         <v>36</v>
       </c>
-      <c r="D76" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B78" t="s">
+      <c r="E78" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B80" s="2"/>
+      <c r="C80" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="11"/>
+      <c r="C82" t="s">
         <v>35</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D82" t="s">
         <v>34</v>
       </c>
-      <c r="D78" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B79" t="s">
+      <c r="E82" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="11"/>
+      <c r="C83" t="s">
         <v>33</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D83" t="s">
         <v>32</v>
       </c>
-      <c r="D79" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B80" t="s">
+      <c r="E83" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="11"/>
+      <c r="C84" t="s">
         <v>31</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D84" t="s">
         <v>30</v>
       </c>
-      <c r="D80" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B81" t="s">
+      <c r="E84" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="11"/>
+      <c r="C85" t="s">
         <v>29</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D85" t="s">
         <v>28</v>
       </c>
-      <c r="D81" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="83" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B83" s="2" t="s">
+      <c r="E85" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B87" s="2"/>
+      <c r="C87" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B85" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C89" t="s">
         <v>26</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D89" t="s">
         <v>25</v>
       </c>
-      <c r="D85" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B86" t="s">
+      <c r="E89" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
         <v>24</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D90" t="s">
         <v>23</v>
       </c>
-      <c r="D86" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B87" t="s">
+      <c r="E90" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C91" t="s">
         <v>23</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D91" t="s">
         <v>22</v>
       </c>
-      <c r="D87" t="s">
+      <c r="E91" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B88" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C92" t="s">
         <v>21</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D92" t="s">
         <v>20</v>
       </c>
-      <c r="D88" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B89" t="s">
+      <c r="E92" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C93" t="s">
         <v>20</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D93" t="s">
         <v>19</v>
       </c>
-      <c r="D89" t="s">
+      <c r="E93" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B90" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C94" t="s">
         <v>18</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D94" t="s">
         <v>17</v>
       </c>
-      <c r="D90" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B91" t="s">
+      <c r="E94" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C95" t="s">
         <v>17</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D95" t="s">
         <v>16</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E95" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B92" t="s">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C96" t="s">
         <v>14</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D96" t="s">
         <v>13</v>
       </c>
-      <c r="D92" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B98" t="s">
+      <c r="E96" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C102" t="s">
         <v>11</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D102" t="s">
         <v>12</v>
       </c>
-      <c r="D98" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B99" t="s">
+      <c r="E102" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C103" t="s">
         <v>11</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D103" t="s">
         <v>11</v>
       </c>
-      <c r="D99" s="3" t="s">
+      <c r="E103" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B101" t="s">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C105" t="s">
         <v>8</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D105" t="s">
         <v>10</v>
       </c>
-      <c r="D101" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B102" t="s">
+      <c r="E105" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C106" t="s">
         <v>8</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D106" t="s">
         <v>8</v>
       </c>
-      <c r="D102" s="3" t="s">
+      <c r="E106" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D103" s="3"/>
-    </row>
-    <row r="104" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B104" s="2" t="s">
+    <row r="107" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E107" s="3"/>
+    </row>
+    <row r="108" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B108" s="2"/>
+      <c r="C108" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B106" t="s">
+    <row r="110" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C110" t="s">
         <v>5</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D110" t="s">
         <v>4</v>
       </c>
-      <c r="D106" t="s">
+      <c r="E110" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C107" t="s">
+    <row r="111" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D111" t="s">
         <v>3</v>
       </c>
-      <c r="D107" t="s">
+      <c r="E111" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B109" t="s">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C113" t="s">
         <v>2</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D113" t="s">
         <v>1</v>
       </c>
-      <c r="D109" t="s">
+      <c r="E113" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C110" t="s">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D114" t="s">
         <v>133</v>
       </c>
-      <c r="D110" t="s">
+      <c r="E114" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B118" s="2" t="s">
+    <row r="122" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B122" s="2"/>
+      <c r="C122" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A120" s="11"/>
-      <c r="B120" t="s">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" s="11"/>
+      <c r="C124" t="s">
         <v>135</v>
       </c>
-      <c r="C120" t="s">
+      <c r="D124" t="s">
         <v>136</v>
       </c>
-      <c r="D120" t="s">
+      <c r="E124" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B123" s="2" t="s">
+    <row r="127" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B127" s="2"/>
+      <c r="C127" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B125" t="s">
+    <row r="129" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C129" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B126" t="s">
+    <row r="130" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C130" t="s">
         <v>141</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated status of refactorings.
</commit_message>
<xml_diff>
--- a/doc/refactoring-3.6.x-to-4.0.0/Refactorings 3.6.x to 4.0.0.xlsx
+++ b/doc/refactoring-3.6.x-to-4.0.0/Refactorings 3.6.x to 4.0.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fries/Documents/Development/Repositories/finmath lib/doc/refactoring-3.6.x-to-4.0.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92033D6-0F71-DC4E-9EC7-0994668A2AA4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FF6904-4A03-2542-8C9A-8E3AC6230ED0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20000" xr2:uid="{89A50B95-A836-9647-8368-30876D9BFE05}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="172">
   <si>
     <t>method</t>
   </si>
@@ -156,9 +156,6 @@
     <t>interface</t>
   </si>
   <si>
-    <t>LIBORCovarianceModelParametric (extract interface)</t>
-  </si>
-  <si>
     <t>AbstractLIBORCovarianceModel</t>
   </si>
   <si>
@@ -622,13 +619,34 @@
   </si>
   <si>
     <t>package</t>
+  </si>
+  <si>
+    <t>TermStructureMonteCarloProduct</t>
+  </si>
+  <si>
+    <t>signature?</t>
+  </si>
+  <si>
+    <t>net.finmath.montecarlo.interestrate.models.modelplugins</t>
+  </si>
+  <si>
+    <t>net.finmath.montecarlo.interestrate.modelplugins</t>
+  </si>
+  <si>
+    <t>LIBORCovarianceModelCalibrateable (extract interface)</t>
+  </si>
+  <si>
+    <t>HybridAssetLIBORModelMonteCarloSimulation</t>
+  </si>
+  <si>
+    <t>HybridAssetLIBORModelMonteCarloSimulationFromModels</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -685,6 +703,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -752,7 +777,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -769,6 +794,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1083,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6EACCA-7E26-C148-ACB1-915E31E23464}">
-  <dimension ref="A1:G139"/>
+  <dimension ref="A1:G143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1103,19 +1129,19 @@
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -1126,7 +1152,7 @@
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="14"/>
       <c r="C3" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1134,13 +1160,13 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>9</v>
@@ -1149,13 +1175,13 @@
     <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
       <c r="B6" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>9</v>
@@ -1163,10 +1189,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>9</v>
@@ -1174,10 +1200,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>9</v>
@@ -1186,25 +1212,25 @@
     <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="14"/>
       <c r="C9" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
       <c r="B10" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>9</v>
@@ -1213,13 +1239,13 @@
     <row r="11" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>9</v>
@@ -1228,13 +1254,13 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>9</v>
@@ -1243,13 +1269,13 @@
     <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>9</v>
@@ -1257,10 +1283,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>9</v>
@@ -1269,10 +1295,10 @@
     <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="14"/>
       <c r="C15" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>9</v>
@@ -1281,13 +1307,13 @@
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>9</v>
@@ -1296,28 +1322,28 @@
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
+        <v>154</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>156</v>
-      </c>
       <c r="E17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>9</v>
@@ -1326,317 +1352,317 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="B19" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C19" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>158</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="14"/>
       <c r="C20" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11"/>
       <c r="B21" s="14"/>
       <c r="C21" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="11"/>
       <c r="B22" s="14"/>
       <c r="C22" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="14"/>
-      <c r="C24" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="C26" t="s">
+    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="11"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="14"/>
+      <c r="C25" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="D26" t="s">
-        <v>93</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="B27" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C27" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
         <v>91</v>
-      </c>
-      <c r="D27" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" t="s">
         <v>89</v>
       </c>
-      <c r="D28" t="s">
-        <v>88</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E28" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="C29" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" t="s">
         <v>87</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="E29" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="11"/>
+      <c r="B30" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="11"/>
-      <c r="B31" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D30" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D31" t="s">
-        <v>84</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E30" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
       <c r="B32" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="C32" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" t="s">
         <v>83</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="E32" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="11"/>
+      <c r="B33" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="D33" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="14"/>
-      <c r="C34" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="11"/>
-      <c r="B36" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="C36" t="s">
-        <v>137</v>
-      </c>
-      <c r="D36" t="s">
-        <v>138</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" t="s">
-        <v>154</v>
+    <row r="35" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="14"/>
+      <c r="C35" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
       <c r="B37" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C37" t="s">
+        <v>136</v>
+      </c>
+      <c r="D37" t="s">
+        <v>137</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" t="s">
         <v>153</v>
-      </c>
-      <c r="C37" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" t="s">
-        <v>75</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
       <c r="B38" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D38" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G38" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
       <c r="B39" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C39" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D39" t="s">
+        <v>71</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="11"/>
+      <c r="B40" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C40" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G39" t="s">
+      <c r="D40" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E40" s="4"/>
-    </row>
-    <row r="42" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="14"/>
-      <c r="C42" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="15"/>
-      <c r="C44" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="D44" s="14" t="s">
+      <c r="E40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E41" s="4"/>
+    </row>
+    <row r="43" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="14"/>
+      <c r="C43" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E44" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="11"/>
-      <c r="B45" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="C45" t="s">
-        <v>75</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="A45" s="15"/>
+      <c r="C45" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="E45" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="11"/>
+      <c r="B46" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="C46" t="s">
         <v>74</v>
       </c>
-      <c r="E45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="13"/>
-      <c r="B46" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="C46" t="s">
-        <v>159</v>
-      </c>
       <c r="D46" t="s">
-        <v>159</v>
+        <v>73</v>
       </c>
       <c r="E46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="13"/>
       <c r="B47" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C47" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="D47" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="E47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="13"/>
       <c r="B48" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C48" t="s">
-        <v>163</v>
+        <v>69</v>
       </c>
       <c r="D48" t="s">
-        <v>163</v>
+        <v>69</v>
       </c>
       <c r="E48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="13"/>
       <c r="B49" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C49" t="s">
         <v>162</v>
@@ -1645,41 +1671,44 @@
         <v>162</v>
       </c>
       <c r="E49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="13"/>
       <c r="B50" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C50" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D50" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E50" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="11"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="11"/>
-      <c r="C54" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="13"/>
+      <c r="B51" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="C51" t="s">
+        <v>163</v>
+      </c>
+      <c r="D51" t="s">
+        <v>163</v>
+      </c>
+      <c r="E51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="11"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="D54" t="s">
-        <v>67</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -1688,45 +1717,45 @@
         <v>67</v>
       </c>
       <c r="D55" t="s">
-        <v>142</v>
-      </c>
-      <c r="E55" t="s">
-        <v>15</v>
+        <v>66</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="11"/>
       <c r="C56" t="s">
-        <v>143</v>
+        <v>66</v>
       </c>
       <c r="D56" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="11"/>
       <c r="C57" t="s">
-        <v>66</v>
+        <v>142</v>
       </c>
       <c r="D57" t="s">
+        <v>143</v>
+      </c>
+      <c r="E57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="11"/>
+      <c r="C58" t="s">
         <v>65</v>
       </c>
-      <c r="E57" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="11"/>
-      <c r="C59" t="s">
+      <c r="D58" t="s">
         <v>64</v>
       </c>
-      <c r="D59" t="s">
-        <v>63</v>
-      </c>
-      <c r="E59" s="4" t="s">
+      <c r="E58" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1738,20 +1767,20 @@
       <c r="D60" t="s">
         <v>62</v>
       </c>
-      <c r="E60" t="s">
-        <v>15</v>
+      <c r="E60" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="11"/>
       <c r="C61" t="s">
+        <v>62</v>
+      </c>
+      <c r="D61" t="s">
         <v>61</v>
       </c>
-      <c r="D61" t="s">
-        <v>60</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>9</v>
+      <c r="E61" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -1762,59 +1791,59 @@
       <c r="D62" t="s">
         <v>59</v>
       </c>
-      <c r="E62" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="11"/>
-      <c r="C64" t="s">
+      <c r="E62" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="11"/>
+      <c r="C63" t="s">
+        <v>59</v>
+      </c>
+      <c r="D63" t="s">
         <v>58</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E63" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="11"/>
+      <c r="C65" t="s">
         <v>57</v>
       </c>
-      <c r="E64" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B66" s="14"/>
-      <c r="C66" s="2" t="s">
+      <c r="D65" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="11"/>
-      <c r="C68" t="s">
+      <c r="E65" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="14"/>
+      <c r="C67" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D68" t="s">
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="11"/>
+      <c r="C69" t="s">
         <v>54</v>
       </c>
-      <c r="E68" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E69" s="4"/>
-    </row>
-    <row r="70" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="14"/>
-      <c r="C70" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="11"/>
-      <c r="C72" t="s">
+      <c r="D69" t="s">
         <v>53</v>
       </c>
-      <c r="D72" t="s">
-        <v>52</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>9</v>
+      <c r="E69" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E70" s="4"/>
+    </row>
+    <row r="71" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="14"/>
+      <c r="C71" s="2" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -1825,50 +1854,50 @@
       <c r="D73" t="s">
         <v>51</v>
       </c>
-      <c r="E73" t="s">
-        <v>15</v>
-      </c>
-      <c r="F73" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="11"/>
-      <c r="C75" t="s">
-        <v>49</v>
-      </c>
-      <c r="D75" t="s">
+      <c r="E73" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="11"/>
+      <c r="C74" t="s">
+        <v>51</v>
+      </c>
+      <c r="D74" t="s">
         <v>50</v>
       </c>
-      <c r="E75" s="4" t="s">
-        <v>9</v>
+      <c r="E74" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="11"/>
       <c r="C76" t="s">
+        <v>48</v>
+      </c>
+      <c r="D76" t="s">
         <v>49</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="11"/>
+      <c r="C77" t="s">
         <v>48</v>
       </c>
-      <c r="E76" t="s">
-        <v>15</v>
-      </c>
-      <c r="F76" t="s">
+      <c r="D77" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="11"/>
-      <c r="C78" t="s">
+      <c r="E77" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" t="s">
         <v>46</v>
-      </c>
-      <c r="D78" t="s">
-        <v>45</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -1879,20 +1908,20 @@
       <c r="D79" t="s">
         <v>44</v>
       </c>
-      <c r="E79" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" s="11"/>
-      <c r="C81" t="s">
+      <c r="E79" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="11"/>
+      <c r="C80" t="s">
+        <v>44</v>
+      </c>
+      <c r="D80" t="s">
         <v>43</v>
       </c>
-      <c r="D81" t="s">
-        <v>42</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>9</v>
+      <c r="E80" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -1903,20 +1932,20 @@
       <c r="D82" t="s">
         <v>41</v>
       </c>
-      <c r="E82" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" s="11"/>
-      <c r="C84" t="s">
+      <c r="E82" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="11"/>
+      <c r="C83" t="s">
+        <v>41</v>
+      </c>
+      <c r="D83" t="s">
         <v>40</v>
       </c>
-      <c r="D84" t="s">
-        <v>39</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>9</v>
+      <c r="E83" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -1927,47 +1956,47 @@
       <c r="D85" t="s">
         <v>38</v>
       </c>
-      <c r="E85" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" s="11"/>
-      <c r="C87" t="s">
+      <c r="E85" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="11"/>
+      <c r="C86" t="s">
+        <v>38</v>
+      </c>
+      <c r="D86" t="s">
         <v>37</v>
       </c>
-      <c r="D87" t="s">
+      <c r="E86" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="11"/>
+      <c r="C88" t="s">
         <v>36</v>
       </c>
-      <c r="E87" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B89" s="14"/>
-      <c r="C89" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" s="11"/>
-      <c r="C91" t="s">
+      <c r="D88" t="s">
         <v>35</v>
       </c>
-      <c r="D91" t="s">
-        <v>34</v>
-      </c>
-      <c r="E91" s="4" t="s">
-        <v>9</v>
+      <c r="E88" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B90" s="14"/>
+      <c r="C90" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="11"/>
       <c r="C92" t="s">
+        <v>34</v>
+      </c>
+      <c r="D92" t="s">
         <v>33</v>
-      </c>
-      <c r="D92" t="s">
-        <v>32</v>
       </c>
       <c r="E92" s="4" t="s">
         <v>9</v>
@@ -1976,10 +2005,10 @@
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="11"/>
       <c r="C93" t="s">
+        <v>32</v>
+      </c>
+      <c r="D93" t="s">
         <v>31</v>
-      </c>
-      <c r="D93" t="s">
-        <v>30</v>
       </c>
       <c r="E93" s="4" t="s">
         <v>9</v>
@@ -1988,232 +2017,269 @@
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="11"/>
       <c r="C94" t="s">
+        <v>30</v>
+      </c>
+      <c r="D94" t="s">
         <v>29</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="11"/>
+      <c r="C95" t="s">
         <v>28</v>
       </c>
-      <c r="E94" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B96" s="14"/>
-      <c r="C96" s="2" t="s">
+      <c r="D95" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="98" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C98" t="s">
+      <c r="E95" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B97" s="14"/>
+      <c r="C97" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D98" t="s">
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C99" t="s">
         <v>25</v>
       </c>
-      <c r="E98" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="99" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C99" t="s">
+      <c r="D99" t="s">
         <v>24</v>
       </c>
-      <c r="D99" t="s">
-        <v>23</v>
-      </c>
       <c r="E99" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C100" t="s">
         <v>23</v>
       </c>
       <c r="D100" t="s">
         <v>22</v>
       </c>
-      <c r="E100" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="101" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E100" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C101" t="s">
+        <v>22</v>
+      </c>
+      <c r="D101" t="s">
         <v>21</v>
       </c>
-      <c r="D101" t="s">
-        <v>20</v>
-      </c>
-      <c r="E101" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="102" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E101" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C102" t="s">
         <v>20</v>
       </c>
       <c r="D102" t="s">
         <v>19</v>
       </c>
-      <c r="E102" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="103" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E102" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C103" t="s">
+        <v>19</v>
+      </c>
+      <c r="D103" t="s">
         <v>18</v>
       </c>
-      <c r="D103" t="s">
-        <v>17</v>
-      </c>
-      <c r="E103" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="104" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C104" t="s">
         <v>17</v>
       </c>
       <c r="D104" t="s">
         <v>16</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E104" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C105" t="s">
+        <v>16</v>
+      </c>
+      <c r="D105" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="105" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C105" t="s">
-        <v>14</v>
-      </c>
-      <c r="D105" t="s">
+      <c r="E105" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C106" t="s">
         <v>13</v>
       </c>
-      <c r="E105" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="111" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D106" t="s">
+        <v>12</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="11"/>
       <c r="C111" t="s">
-        <v>11</v>
+        <v>168</v>
       </c>
       <c r="D111" t="s">
-        <v>12</v>
-      </c>
-      <c r="E111" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="112" spans="3:5" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="11"/>
+      <c r="B112" s="14" t="s">
+        <v>167</v>
+      </c>
       <c r="C112" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D112" t="s">
         <v>11</v>
       </c>
-      <c r="E112" s="3" t="s">
+      <c r="E112" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="11"/>
+      <c r="C113" t="s">
+        <v>10</v>
+      </c>
+      <c r="D113" t="s">
+        <v>10</v>
+      </c>
+      <c r="E113" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C114" t="s">
-        <v>8</v>
-      </c>
-      <c r="D114" t="s">
-        <v>10</v>
-      </c>
-      <c r="E114" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="11"/>
       <c r="C115" t="s">
         <v>8</v>
       </c>
       <c r="D115" t="s">
+        <v>169</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" s="11"/>
+      <c r="C116" t="s">
         <v>8</v>
       </c>
-      <c r="E115" s="3" t="s">
+      <c r="D116" t="s">
+        <v>8</v>
+      </c>
+      <c r="E116" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E116" s="3"/>
-    </row>
-    <row r="117" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B117" s="14"/>
-      <c r="C117" s="2" t="s">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E117" s="3"/>
+    </row>
+    <row r="118" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B118" s="14"/>
+      <c r="C118" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C119" t="s">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" s="11"/>
+      <c r="C120" t="s">
         <v>5</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D120" t="s">
         <v>4</v>
-      </c>
-      <c r="E119" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D120" t="s">
-        <v>3</v>
       </c>
       <c r="E120" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C122" t="s">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D121" t="s">
+        <v>3</v>
+      </c>
+      <c r="E121" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C123" t="s">
         <v>2</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D123" t="s">
         <v>1</v>
-      </c>
-      <c r="E122" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D123" t="s">
-        <v>133</v>
       </c>
       <c r="E123" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B131" s="14"/>
-      <c r="C131" s="2" t="s">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D124" t="s">
+        <v>132</v>
+      </c>
+      <c r="E124" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B132" s="14"/>
+      <c r="C132" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" s="11"/>
+      <c r="C134" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A133" s="11"/>
-      <c r="C133" t="s">
+      <c r="D134" t="s">
         <v>135</v>
       </c>
-      <c r="D133" t="s">
-        <v>136</v>
-      </c>
-      <c r="E133" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B136" s="14"/>
-      <c r="C136" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C138" t="s">
+      <c r="E134" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B137" s="14"/>
+      <c r="C137" s="2" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C139" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C140" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C143" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="E143" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added additional refactorings for ParameterObject(Interface).
</commit_message>
<xml_diff>
--- a/doc/refactoring-3.6.x-to-4.0.0/Refactorings 3.6.x to 4.0.0.xlsx
+++ b/doc/refactoring-3.6.x-to-4.0.0/Refactorings 3.6.x to 4.0.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fries/Documents/Development/Repositories/finmath lib/doc/refactoring-3.6.x-to-4.0.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA34C8E-BC94-8349-A577-76C04F4DAF10}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF41D7A3-E5DD-1E46-9C66-C8FA945C1A4A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="460" windowWidth="33600" windowHeight="19980" xr2:uid="{89A50B95-A836-9647-8368-30876D9BFE05}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19980" xr2:uid="{89A50B95-A836-9647-8368-30876D9BFE05}"/>
   </bookViews>
   <sheets>
     <sheet name="Refactorings 3.x to 4.x" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="177">
   <si>
     <t>method</t>
   </si>
@@ -649,6 +649,12 @@
   </si>
   <si>
     <t>AbstractFourierTransformProduct (Interface)</t>
+  </si>
+  <si>
+    <t>ParameterObjectInterface</t>
+  </si>
+  <si>
+    <t>ParameterObject</t>
   </si>
 </sst>
 </file>
@@ -1120,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6EACCA-7E26-C148-ACB1-915E31E23464}">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C139" sqref="C139"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2191,6 +2197,18 @@
         <v>9</v>
       </c>
     </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="11"/>
+      <c r="C111" t="s">
+        <v>175</v>
+      </c>
+      <c r="D111" t="s">
+        <v>176</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="11"/>
       <c r="C114" t="s">

</xml_diff>

<commit_message>
Refactoring: Extracted interface ShortRateVolatilityModelParametric.
</commit_message>
<xml_diff>
--- a/doc/refactoring-3.6.x-to-4.0.0/Refactorings 3.6.x to 4.0.0.xlsx
+++ b/doc/refactoring-3.6.x-to-4.0.0/Refactorings 3.6.x to 4.0.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fries/Documents/Development/Repositories/finmath lib/doc/refactoring-3.6.x-to-4.0.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF41D7A3-E5DD-1E46-9C66-C8FA945C1A4A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C045E0A-7DBF-D84B-97E6-3E5C5675E01D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19980" xr2:uid="{89A50B95-A836-9647-8368-30876D9BFE05}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="186">
   <si>
     <t>method</t>
   </si>
@@ -655,6 +655,33 @@
   </si>
   <si>
     <t>ParameterObject</t>
+  </si>
+  <si>
+    <t>Forward Rate Models: Volatility Models</t>
+  </si>
+  <si>
+    <t>AbstractShortRateVolatilityModel</t>
+  </si>
+  <si>
+    <t>ShortRateVolatilityModelInterface</t>
+  </si>
+  <si>
+    <t>AbstractShortRateVolatilityModelParametric</t>
+  </si>
+  <si>
+    <t>ShortRateVolatilityModelCalibrateable</t>
+  </si>
+  <si>
+    <t>ShortRateVolatilityModelParametric (extract interface)</t>
+  </si>
+  <si>
+    <t>double[] AbstractShortRateVolatilityModelParametric.getParameter()</t>
+  </si>
+  <si>
+    <t>double[] AbstractShortRateVolatilityModelParametric.getParameterAsDouble()</t>
+  </si>
+  <si>
+    <t>RandomVariable[] AbstractShortRateVolatilityModelParametric.getParameter()</t>
   </si>
 </sst>
 </file>
@@ -1124,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6EACCA-7E26-C148-ACB1-915E31E23464}">
-  <dimension ref="A1:G140"/>
+  <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2209,52 +2236,46 @@
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A114" s="11"/>
-      <c r="C114" t="s">
-        <v>166</v>
-      </c>
-      <c r="D114" t="s">
-        <v>165</v>
+    <row r="113" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B113" s="14"/>
+      <c r="C113" s="2" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="11"/>
-      <c r="B115" s="14" t="s">
+      <c r="C115" t="s">
+        <v>166</v>
+      </c>
+      <c r="D115" t="s">
         <v>165</v>
-      </c>
-      <c r="C115" t="s">
-        <v>10</v>
-      </c>
-      <c r="D115" t="s">
-        <v>11</v>
-      </c>
-      <c r="E115" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="11"/>
+      <c r="B116" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="C116" t="s">
         <v>10</v>
       </c>
       <c r="D116" t="s">
+        <v>11</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" s="11"/>
+      <c r="C117" t="s">
         <v>10</v>
       </c>
-      <c r="E116" s="3" t="s">
+      <c r="D117" t="s">
+        <v>10</v>
+      </c>
+      <c r="E117" s="3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A118" s="11"/>
-      <c r="C118" t="s">
-        <v>8</v>
-      </c>
-      <c r="D118" t="s">
-        <v>167</v>
-      </c>
-      <c r="E118" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -2263,91 +2284,200 @@
         <v>8</v>
       </c>
       <c r="D119" t="s">
+        <v>167</v>
+      </c>
+      <c r="E119" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" s="11"/>
+      <c r="C120" t="s">
         <v>8</v>
       </c>
-      <c r="E119" s="3" t="s">
+      <c r="D120" t="s">
+        <v>8</v>
+      </c>
+      <c r="E120" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E120" s="3"/>
-    </row>
-    <row r="121" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B121" s="14"/>
-      <c r="C121" s="2" t="s">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E121" s="3"/>
+    </row>
+    <row r="122" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B122" s="14"/>
+      <c r="C122" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E123" s="3"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" s="13"/>
+      <c r="C124" t="s">
+        <v>179</v>
+      </c>
+      <c r="D124" t="s">
+        <v>179</v>
+      </c>
+      <c r="E124" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125" s="13"/>
+      <c r="C125" t="s">
+        <v>178</v>
+      </c>
+      <c r="D125" t="s">
+        <v>178</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E126" s="3"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" s="11"/>
+      <c r="C127" t="s">
+        <v>180</v>
+      </c>
+      <c r="D127" t="s">
+        <v>182</v>
+      </c>
+      <c r="E127" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128" s="13"/>
+      <c r="C128" t="s">
+        <v>180</v>
+      </c>
+      <c r="D128" t="s">
+        <v>180</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129" s="13"/>
+      <c r="C129" t="s">
+        <v>181</v>
+      </c>
+      <c r="D129" t="s">
+        <v>181</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E130" s="3"/>
+    </row>
+    <row r="131" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B131" s="14"/>
+      <c r="C131" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A123" s="11"/>
-      <c r="C123" t="s">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133" s="11"/>
+      <c r="C133" t="s">
         <v>5</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D133" t="s">
         <v>4</v>
       </c>
-      <c r="E123" t="s">
+      <c r="E133" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D124" t="s">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134" s="11"/>
+      <c r="D134" t="s">
         <v>3</v>
       </c>
-      <c r="E124" t="s">
+      <c r="E134" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C126" t="s">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136" s="11"/>
+      <c r="C136" t="s">
+        <v>183</v>
+      </c>
+      <c r="D136" t="s">
+        <v>184</v>
+      </c>
+      <c r="E136" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137" s="11"/>
+      <c r="D137" t="s">
+        <v>185</v>
+      </c>
+      <c r="E137" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C139" t="s">
         <v>2</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D139" t="s">
         <v>1</v>
       </c>
-      <c r="E126" t="s">
+      <c r="E139" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B129" s="14"/>
-      <c r="C129" s="2" t="s">
+    <row r="142" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B142" s="14"/>
+      <c r="C142" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A131" s="11"/>
-      <c r="C131" t="s">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144" s="11"/>
+      <c r="C144" t="s">
         <v>132</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D144" t="s">
         <v>133</v>
       </c>
-      <c r="E131" t="s">
+      <c r="E144" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="134" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B134" s="14"/>
-      <c r="C134" s="2" t="s">
+    <row r="147" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B147" s="14"/>
+      <c r="C147" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C136" t="s">
+    <row r="149" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C149" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C137" t="s">
+    <row r="150" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C150" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C140" s="16" t="s">
+    <row r="153" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C153" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E153" t="s">
         <v>164</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactoring. Renamed class name.
Small adjustment to improve consistency of last refactoring session:
`CurveFromInterpolationPoints` renamed to `CurveInterpolation`.

Clean up.
</commit_message>
<xml_diff>
--- a/doc/refactoring-3.6.x-to-4.0.0/Refactorings 3.6.x to 4.0.0.xlsx
+++ b/doc/refactoring-3.6.x-to-4.0.0/Refactorings 3.6.x to 4.0.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fries/Documents/Development/Repositories/finmath lib/doc/refactoring-3.6.x-to-4.0.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2779B7FE-2379-4245-BDE7-69B68F4F6A24}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4351AC93-4D8B-0A46-AF78-89AE8B8471DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19980" xr2:uid="{89A50B95-A836-9647-8368-30876D9BFE05}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="191">
   <si>
     <t>method</t>
   </si>
@@ -189,9 +189,6 @@
     <t>DiscountCurveInterface</t>
   </si>
   <si>
-    <t>CurveFromInterpolationPoints</t>
-  </si>
-  <si>
     <t>Curve</t>
   </si>
   <si>
@@ -618,9 +615,6 @@
     <t>signature?</t>
   </si>
   <si>
-    <t>net.finmath.montecarlo.interestrate.models.modelplugins</t>
-  </si>
-  <si>
     <t>net.finmath.montecarlo.interestrate.modelplugins</t>
   </si>
   <si>
@@ -688,6 +682,21 @@
   </si>
   <si>
     <t>AnalyticModelFromCurvesAndVols</t>
+  </si>
+  <si>
+    <t>net.finmath.montecarlo.interestrate.models.covariance</t>
+  </si>
+  <si>
+    <t>net.finmath.stochastic</t>
+  </si>
+  <si>
+    <t>net.finmath.fouriermethod</t>
+  </si>
+  <si>
+    <t>net.finmath.marketdata</t>
+  </si>
+  <si>
+    <t>CurveInterpolation</t>
   </si>
 </sst>
 </file>
@@ -1175,19 +1184,19 @@
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -1196,9 +1205,9 @@
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="14"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1206,13 +1215,13 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>9</v>
@@ -1221,13 +1230,13 @@
     <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
       <c r="B6" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>9</v>
@@ -1235,11 +1244,14 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
+      <c r="B7" s="14" t="s">
+        <v>189</v>
+      </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>9</v>
@@ -1247,11 +1259,14 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
+      <c r="B8" s="14" t="s">
+        <v>189</v>
+      </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>9</v>
@@ -1259,12 +1274,14 @@
     </row>
     <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
-      <c r="B9" s="14"/>
+      <c r="B9" s="14" t="s">
+        <v>189</v>
+      </c>
       <c r="C9" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>14</v>
@@ -1273,13 +1290,13 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
       <c r="B10" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>9</v>
@@ -1288,13 +1305,13 @@
     <row r="11" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>9</v>
@@ -1303,13 +1320,13 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>9</v>
@@ -1318,13 +1335,13 @@
     <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>9</v>
@@ -1332,12 +1349,14 @@
     </row>
     <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
-      <c r="B14" s="14"/>
+      <c r="B14" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="C14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>9</v>
@@ -1345,11 +1364,14 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
+      <c r="B15" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="C15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>9</v>
@@ -1357,11 +1379,14 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
+      <c r="B16" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="C16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D16" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>9</v>
@@ -1369,12 +1394,14 @@
     </row>
     <row r="17" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
-      <c r="B17" s="14"/>
+      <c r="B17" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="C17" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>7</v>
@@ -1383,13 +1410,13 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>9</v>
@@ -1398,13 +1425,13 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="B19" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>151</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>152</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>14</v>
@@ -1413,13 +1440,13 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>9</v>
@@ -1428,13 +1455,13 @@
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
       <c r="B21" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C21" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>153</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>154</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>14</v>
@@ -1444,10 +1471,10 @@
       <c r="A22" s="11"/>
       <c r="B22" s="14"/>
       <c r="C22" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>9</v>
@@ -1457,10 +1484,10 @@
       <c r="A23" s="11"/>
       <c r="B23" s="14"/>
       <c r="C23" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>9</v>
@@ -1470,10 +1497,10 @@
       <c r="A24" s="11"/>
       <c r="B24" s="14"/>
       <c r="C24" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>9</v>
@@ -1483,49 +1510,49 @@
       <c r="A25" s="11"/>
       <c r="B25" s="14"/>
       <c r="C25" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="14"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
       <c r="B30" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>9</v>
@@ -1534,13 +1561,13 @@
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="B31" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>7</v>
@@ -1549,13 +1576,13 @@
     <row r="32" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
       <c r="B32" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>14</v>
@@ -1564,13 +1591,13 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
       <c r="B34" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>9</v>
@@ -1579,127 +1606,127 @@
     <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
       <c r="B35" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="14"/>
+      <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
       <c r="B39" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39" t="s">
+        <v>133</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" t="s">
         <v>149</v>
-      </c>
-      <c r="C39" t="s">
-        <v>133</v>
-      </c>
-      <c r="D39" t="s">
-        <v>134</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
       <c r="B40" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D40" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" t="s">
         <v>74</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="11"/>
       <c r="B41" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
       <c r="B42" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E43" s="4"/>
     </row>
     <row r="45" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="14"/>
+      <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="15"/>
       <c r="C47" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E47" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
       <c r="B48" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E48" t="s">
         <v>14</v>
@@ -1708,13 +1735,13 @@
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="13"/>
       <c r="B49" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C49" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D49" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E49" t="s">
         <v>14</v>
@@ -1723,13 +1750,13 @@
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="13"/>
       <c r="B50" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E50" t="s">
         <v>14</v>
@@ -1738,13 +1765,13 @@
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="13"/>
       <c r="B51" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E51" t="s">
         <v>14</v>
@@ -1753,13 +1780,13 @@
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="13"/>
       <c r="B52" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C52" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D52" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E52" t="s">
         <v>14</v>
@@ -1768,13 +1795,13 @@
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="13"/>
       <c r="B53" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C53" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D53" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E53" t="s">
         <v>14</v>
@@ -1782,18 +1809,21 @@
     </row>
     <row r="55" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="11"/>
-      <c r="B55" s="14"/>
+      <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="11"/>
+      <c r="B57" s="14" t="s">
+        <v>187</v>
+      </c>
       <c r="C57" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>9</v>
@@ -1801,11 +1831,14 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="11"/>
+      <c r="B58" s="14" t="s">
+        <v>145</v>
+      </c>
       <c r="C58" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E58" t="s">
         <v>14</v>
@@ -1813,11 +1846,14 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="11"/>
+      <c r="B59" s="14" t="s">
+        <v>145</v>
+      </c>
       <c r="C59" t="s">
+        <v>138</v>
+      </c>
+      <c r="D59" t="s">
         <v>139</v>
-      </c>
-      <c r="D59" t="s">
-        <v>140</v>
       </c>
       <c r="E59" t="s">
         <v>14</v>
@@ -1825,11 +1861,14 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="11"/>
+      <c r="B60" s="14" t="s">
+        <v>145</v>
+      </c>
       <c r="C60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>9</v>
@@ -1837,11 +1876,14 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="11"/>
+      <c r="B62" s="14" t="s">
+        <v>145</v>
+      </c>
       <c r="C62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>9</v>
@@ -1849,11 +1891,14 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="11"/>
+      <c r="B63" s="14" t="s">
+        <v>145</v>
+      </c>
       <c r="C63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E63" t="s">
         <v>14</v>
@@ -1861,11 +1906,14 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="11"/>
+      <c r="B64" s="14" t="s">
+        <v>145</v>
+      </c>
       <c r="C64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>9</v>
@@ -1873,11 +1921,14 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="11"/>
+      <c r="B65" s="14" t="s">
+        <v>145</v>
+      </c>
       <c r="C65" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D65" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E65" t="s">
         <v>14</v>
@@ -1886,28 +1937,28 @@
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="11"/>
       <c r="C67" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D67" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="14"/>
+      <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="11"/>
       <c r="C71" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D71" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>9</v>
@@ -1917,18 +1968,18 @@
       <c r="E72" s="4"/>
     </row>
     <row r="73" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="14"/>
+      <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="11"/>
       <c r="C75" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D75" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>9</v>
@@ -1937,25 +1988,25 @@
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="11"/>
       <c r="C76" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D76" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E76" t="s">
         <v>14</v>
       </c>
       <c r="F76" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="11"/>
       <c r="C78" t="s">
+        <v>47</v>
+      </c>
+      <c r="D78" t="s">
         <v>48</v>
-      </c>
-      <c r="D78" t="s">
-        <v>49</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>9</v>
@@ -1964,25 +2015,25 @@
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="11"/>
       <c r="C79" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D79" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E79" t="s">
         <v>14</v>
       </c>
       <c r="F79" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="11"/>
       <c r="C81" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D81" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>9</v>
@@ -1991,10 +2042,10 @@
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="11"/>
       <c r="C82" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D82" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E82" t="s">
         <v>14</v>
@@ -2003,10 +2054,10 @@
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="11"/>
       <c r="C84" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D84" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>9</v>
@@ -2015,10 +2066,10 @@
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="11"/>
       <c r="C85" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D85" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E85" t="s">
         <v>14</v>
@@ -2027,10 +2078,10 @@
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="11"/>
       <c r="C87" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D87" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>9</v>
@@ -2039,10 +2090,10 @@
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="11"/>
       <c r="C88" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D88" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E88" t="s">
         <v>14</v>
@@ -2051,28 +2102,28 @@
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="11"/>
       <c r="C90" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D90" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B92" s="14"/>
+      <c r="B92" s="2"/>
       <c r="C92" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="11"/>
       <c r="C94" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D94" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E94" s="4" t="s">
         <v>9</v>
@@ -2081,10 +2132,10 @@
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="11"/>
       <c r="C95" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D95" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>9</v>
@@ -2093,10 +2144,10 @@
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="11"/>
       <c r="C96" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D96" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>9</v>
@@ -2105,28 +2156,28 @@
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="11"/>
       <c r="C97" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D97" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E97" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="99" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B99" s="14"/>
+      <c r="B99" s="2"/>
       <c r="C99" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="11"/>
       <c r="C101" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D101" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>9</v>
@@ -2135,10 +2186,10 @@
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="11"/>
       <c r="C102" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D102" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E102" t="s">
         <v>14</v>
@@ -2147,10 +2198,10 @@
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="11"/>
       <c r="C103" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D103" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>9</v>
@@ -2159,10 +2210,10 @@
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="11"/>
       <c r="C104" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D104" t="s">
-        <v>21</v>
+        <v>190</v>
       </c>
       <c r="E104" t="s">
         <v>14</v>
@@ -2231,34 +2282,34 @@
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="11"/>
       <c r="C111" t="s">
+        <v>172</v>
+      </c>
+      <c r="D111" t="s">
+        <v>173</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B113" s="2"/>
+      <c r="C113" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="D111" t="s">
-        <v>175</v>
-      </c>
-      <c r="E111" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B113" s="14"/>
-      <c r="C113" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="11"/>
       <c r="C115" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D115" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="11"/>
       <c r="B116" s="14" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="C116" t="s">
         <v>10</v>
@@ -2272,6 +2323,9 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="11"/>
+      <c r="B117" s="14" t="s">
+        <v>186</v>
+      </c>
       <c r="C117" t="s">
         <v>10</v>
       </c>
@@ -2284,11 +2338,14 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="11"/>
+      <c r="B119" s="14" t="s">
+        <v>186</v>
+      </c>
       <c r="C119" t="s">
         <v>8</v>
       </c>
       <c r="D119" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E119" s="4" t="s">
         <v>9</v>
@@ -2296,6 +2353,9 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="11"/>
+      <c r="B120" s="14" t="s">
+        <v>186</v>
+      </c>
       <c r="C120" t="s">
         <v>8</v>
       </c>
@@ -2310,9 +2370,9 @@
       <c r="E121" s="3"/>
     </row>
     <row r="122" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B122" s="14"/>
+      <c r="B122" s="2"/>
       <c r="C122" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -2320,11 +2380,14 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="13"/>
+      <c r="B124" s="14" t="s">
+        <v>186</v>
+      </c>
       <c r="C124" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D124" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E124" s="4" t="s">
         <v>9</v>
@@ -2332,11 +2395,14 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="13"/>
+      <c r="B125" s="14" t="s">
+        <v>186</v>
+      </c>
       <c r="C125" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D125" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>7</v>
@@ -2347,11 +2413,14 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="11"/>
+      <c r="B127" s="14" t="s">
+        <v>186</v>
+      </c>
       <c r="C127" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D127" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E127" s="4" t="s">
         <v>9</v>
@@ -2359,11 +2428,14 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="11"/>
+      <c r="B128" s="14" t="s">
+        <v>186</v>
+      </c>
       <c r="C128" t="s">
+        <v>177</v>
+      </c>
+      <c r="D128" t="s">
         <v>179</v>
-      </c>
-      <c r="D128" t="s">
-        <v>181</v>
       </c>
       <c r="E128" s="4" t="s">
         <v>9</v>
@@ -2371,11 +2443,14 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="13"/>
+      <c r="B129" s="14" t="s">
+        <v>186</v>
+      </c>
       <c r="C129" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D129" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>7</v>
@@ -2383,11 +2458,14 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="13"/>
+      <c r="B130" s="14" t="s">
+        <v>186</v>
+      </c>
       <c r="C130" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D130" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E130" s="4" t="s">
         <v>9</v>
@@ -2395,11 +2473,14 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="11"/>
+      <c r="B131" s="14" t="s">
+        <v>186</v>
+      </c>
       <c r="C131" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D131" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E131" t="s">
         <v>14</v>
@@ -2412,7 +2493,7 @@
       <c r="E133" s="3"/>
     </row>
     <row r="134" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B134" s="14"/>
+      <c r="B134" s="2"/>
       <c r="C134" s="2" t="s">
         <v>6</v>
       </c>
@@ -2441,10 +2522,10 @@
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="11"/>
       <c r="C139" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D139" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E139" t="s">
         <v>0</v>
@@ -2453,7 +2534,7 @@
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="11"/>
       <c r="D140" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E140" t="s">
         <v>0</v>
@@ -2471,18 +2552,18 @@
       </c>
     </row>
     <row r="145" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B145" s="14"/>
+      <c r="B145" s="2"/>
       <c r="C145" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="11"/>
       <c r="C147" t="s">
+        <v>130</v>
+      </c>
+      <c r="D147" t="s">
         <v>131</v>
-      </c>
-      <c r="D147" t="s">
-        <v>132</v>
       </c>
       <c r="E147" t="s">
         <v>14</v>
@@ -2491,25 +2572,25 @@
     <row r="150" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B150" s="14"/>
       <c r="C150" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C152" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C153" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C156" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="E156" t="s">
         <v>162</v>
-      </c>
-      <c r="E156" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>